<commit_message>
Added blanket exception handler for release. Should be removed for debugging and development. Repopulated Excel document
</commit_message>
<xml_diff>
--- a/periodic_table.xlsx
+++ b/periodic_table.xlsx
@@ -3882,15 +3882,12 @@
 DP
 58Ni
 68.077%
-&gt;7×1020 y
-(β+β+)
-1.9258
-58Fe
+58Ni is stable with 30 neutrons
 59Ni
 trace
 7.6×104 y
 ε
-–
+0.0506
 59Co
 60Ni
 26.223%
@@ -4166,10 +4163,7 @@
 DP
 64Zn
 49.2%
-&gt;2.3×1018 y
-(β+β+)
-1.096
-64Ni
+64Zn is stable with 34 neutrons
 65Zn
 syn
 243.8 d
@@ -4202,10 +4196,7 @@
 69Ga
 70Zn
 0.6%
-&gt;1.3×1016 y
-(β−β−)
-0.998
-70Ge
+70Zn is stable with 40 neutrons
 71Zn
 syn
 2.4 min
@@ -4903,9 +4894,6 @@
     <t>(Br2) 10.571 kJ/mol</t>
   </si>
   <si>
-    <t>(Br2) 29.96 kJ/mol</t>
-  </si>
-  <si>
     <t>(Br2) 75.69 J/(mol·K)</t>
   </si>
   <si>
@@ -4913,11 +4901,6 @@
   </si>
   <si>
     <t>Pauling scale: 2.96</t>
-  </si>
-  <si>
-    <t>1st: 1139.9 kJ/mol
-2nd: 2103 kJ/mol
-3rd: 3470 kJ/mol</t>
   </si>
   <si>
     <t>120±3 pm</t>
@@ -4957,6 +4940,14 @@
     <t>Antoine Jérôme Balard and Leopold Gmelin (1825)</t>
   </si>
   <si>
+    <t>(Br2) 29.96 kJ/mol</t>
+  </si>
+  <si>
+    <t>1st: 1139.9 kJ/mol
+2nd: 2103 kJ/mol
+3rd: 3470 kJ/mol</t>
+  </si>
+  <si>
     <t>Krypton</t>
   </si>
   <si>
@@ -5042,10 +5033,7 @@
 DP
 78Kr
 0.36%
-&gt;1.1×1020 y
-(β+β+)
-2.846
-78Se
+78Kr is stable with 42 neutrons
 79Kr
 syn
 35.04 h
@@ -5087,10 +5075,7 @@
 85Rb
 86Kr
 17.28%
-–
-(β−β−)
-1.2556
-86Sr
+86Kr is stable with 50 neutrons
 </t>
   </si>
   <si>
@@ -5662,19 +5647,13 @@
 93Nb
 94Zr
 17.38%
-&gt;1.1×1017 y
-(β−β−)
-1.144
-94Mo
+94Zr is stable with 54 neutrons
 96Zr
 2.80%
 2.0×1019 y[4]
 β−β−
 3.348
 96Mo
-(β−)
-–
-96Nb
 </t>
   </si>
   <si>
@@ -7440,10 +7419,7 @@
 DP
 120Te
 0.09%
-&gt;2.2×1016 y
-(β+β+)
-1.701
-120Sn
+120Te is stable with 68 neutrons
 121Te
 syn
 16.78 d
@@ -7452,30 +7428,19 @@
 121Sb
 122Te
 2.55%
-–
-(SF)
-&lt;30.974
+122Te is stable with 70 neutrons
 123Te
-0.89%
-&gt;9.2×1016 y[4]
-(ε)
-0.051
-123Sb
+0.89%[4]
+123Te is stable with 71 neutrons
 124Te
 4.74%
-–
-(SF)
-&lt;28.221
+124Te is stable with 72 neutrons
 125Te
 7.07%
-–
-(SF)
-&lt;26.966
+125Te is stable with 73 neutrons
 126Te
 18.84%
-–
-(SF)
-&lt;26.011
+126Te is stable with 74 neutrons
 127Te
 syn
 9.35 h
@@ -8821,8 +8786,8 @@
 –
 145Pm
 146Sm
-trace
-1.03×108 y
+syn
+6.8×107 y
 α
 2.529
 142Nd
@@ -20217,23 +20182,17 @@
       <c r="W36" t="s">
         <v>1234</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>1235</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>1236</v>
       </c>
-      <c r="Z36" t="s">
+      <c r="AA36" t="s">
         <v>1237</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AC36" t="s">
         <v>1238</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>1239</v>
-      </c>
-      <c r="AC36" t="s">
-        <v>1240</v>
       </c>
       <c r="AD36" t="s">
         <v>1172</v>
@@ -20242,30 +20201,36 @@
         <v>608</v>
       </c>
       <c r="AF36" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="AG36" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="AH36" t="s">
         <v>641</v>
       </c>
       <c r="AI36" t="s">
+        <v>1241</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>1242</v>
+      </c>
+      <c r="AP36" t="s">
         <v>1243</v>
-      </c>
-      <c r="AL36" t="s">
-        <v>1244</v>
-      </c>
-      <c r="AP36" t="s">
-        <v>1245</v>
       </c>
       <c r="AQ36" t="s">
         <v>1213</v>
       </c>
       <c r="AT36" t="s">
+        <v>1244</v>
+      </c>
+      <c r="BG36" t="s">
+        <v>1245</v>
+      </c>
+      <c r="BJ36" t="s">
         <v>1246</v>
       </c>
-      <c r="BG36" t="s">
+      <c r="BK36" t="s">
         <v>1247</v>
       </c>
     </row>

</xml_diff>